<commit_message>
se modifica el excel, se añade un txt con ideas de restricciones para ruta critica
</commit_message>
<xml_diff>
--- a/generador ruta critica/MallaCurricular.xlsx
+++ b/generador ruta critica/MallaCurricular.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador ruta critica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C0C450-63FF-4A29-A6C2-10D622FCB18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E32148-5239-4318-9842-32E44E7E1F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="113">
   <si>
     <t>CBM1000</t>
   </si>
@@ -330,52 +330,49 @@
     <t>Nombre Asignatura</t>
   </si>
   <si>
-    <t>Prerrequisito</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>CBM1002 - CBM1003</t>
-  </si>
-  <si>
-    <t>CBM1003 - CBF1000</t>
-  </si>
-  <si>
-    <t>CBM1005 -CBM1006</t>
-  </si>
-  <si>
-    <t>CBM1002 - CBM1006</t>
-  </si>
-  <si>
-    <t>CIT2100 - CIT 2001</t>
-  </si>
-  <si>
-    <t>CIT2100 - CIT2204 - CII2750</t>
-  </si>
-  <si>
-    <t>CIT2204 - CIT2106</t>
-  </si>
-  <si>
-    <t>CIT2100 - CIT2002</t>
-  </si>
-  <si>
-    <t>CIT2200 - CIT2002</t>
-  </si>
-  <si>
-    <t>CIT2200 - CIT2005 - CIT2102</t>
-  </si>
-  <si>
-    <t>CII1000 - CIT2201</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Semestre</t>
   </si>
   <si>
-    <t>NULL</t>
+    <t>Abre la/s asignatura/s:</t>
+  </si>
+  <si>
+    <t>11, 17, 22</t>
+  </si>
+  <si>
+    <t>7, 8, 33</t>
+  </si>
+  <si>
+    <t>11, 12, 13, 16, 17</t>
+  </si>
+  <si>
+    <t>14, 15</t>
+  </si>
+  <si>
+    <t>18, 22, 28</t>
+  </si>
+  <si>
+    <t>24, 29, 31</t>
+  </si>
+  <si>
+    <t>29, 30</t>
+  </si>
+  <si>
+    <t>24, 25</t>
+  </si>
+  <si>
+    <t>30, 32</t>
+  </si>
+  <si>
+    <t>34, 41</t>
+  </si>
+  <si>
+    <t>31, 35</t>
+  </si>
+  <si>
+    <t>39, 41</t>
   </si>
 </sst>
 </file>
@@ -523,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -546,6 +543,16 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -874,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +896,7 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>96</v>
@@ -898,10 +905,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -914,8 +921,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>99</v>
+      <c r="D3" s="22">
+        <v>6</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
@@ -931,8 +938,8 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>99</v>
+      <c r="D4" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
@@ -948,9 +955,7 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="D5" s="22"/>
       <c r="E5" s="12">
         <v>1</v>
       </c>
@@ -965,8 +970,8 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>99</v>
+      <c r="D6" s="22">
+        <v>9</v>
       </c>
       <c r="E6" s="12">
         <v>1</v>
@@ -982,8 +987,8 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>99</v>
+      <c r="D7" s="22">
+        <v>38</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
@@ -999,8 +1004,8 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>0</v>
+      <c r="D8" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="E8" s="13">
         <v>2</v>
@@ -1016,8 +1021,8 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
+      <c r="D9" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="E9" s="13">
         <v>2</v>
@@ -1033,8 +1038,8 @@
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
+      <c r="D10" s="23">
+        <v>13</v>
       </c>
       <c r="E10" s="13">
         <v>2</v>
@@ -1050,8 +1055,8 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>3</v>
+      <c r="D11" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="E11" s="13">
         <v>2</v>
@@ -1067,9 +1072,7 @@
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="D12" s="23"/>
       <c r="E12" s="13">
         <v>2</v>
       </c>
@@ -1084,8 +1087,8 @@
       <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>100</v>
+      <c r="D13" s="24">
+        <v>18</v>
       </c>
       <c r="E13" s="14">
         <v>3</v>
@@ -1101,8 +1104,8 @@
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
+      <c r="D14" s="24" t="s">
+        <v>105</v>
       </c>
       <c r="E14" s="14">
         <v>3</v>
@@ -1118,9 +1121,7 @@
       <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>101</v>
-      </c>
+      <c r="D15" s="24"/>
       <c r="E15" s="14">
         <v>3</v>
       </c>
@@ -1135,8 +1136,8 @@
       <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
+      <c r="D16" s="24">
+        <v>19</v>
       </c>
       <c r="E16" s="14">
         <v>3</v>
@@ -1152,8 +1153,8 @@
       <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
+      <c r="D17" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="E17" s="14">
         <v>3</v>
@@ -1169,8 +1170,8 @@
       <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>11</v>
+      <c r="D18" s="25" t="s">
+        <v>107</v>
       </c>
       <c r="E18" s="15">
         <v>4</v>
@@ -1186,9 +1187,7 @@
       <c r="C19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="D19" s="25"/>
       <c r="E19" s="15">
         <v>4</v>
       </c>
@@ -1203,8 +1202,8 @@
       <c r="C20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>102</v>
+      <c r="D20" s="25">
+        <v>23</v>
       </c>
       <c r="E20" s="15">
         <v>4</v>
@@ -1220,8 +1219,8 @@
       <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>23</v>
+      <c r="D21" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="E21" s="15">
         <v>4</v>
@@ -1237,9 +1236,7 @@
       <c r="C22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="D22" s="25"/>
       <c r="E22" s="15">
         <v>4</v>
       </c>
@@ -1254,8 +1251,8 @@
       <c r="C23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>99</v>
+      <c r="D23" s="25">
+        <v>27</v>
       </c>
       <c r="E23" s="15">
         <v>4</v>
@@ -1271,8 +1268,8 @@
       <c r="C24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>103</v>
+      <c r="D24" s="26">
+        <v>29</v>
       </c>
       <c r="E24" s="16">
         <v>5</v>
@@ -1288,8 +1285,8 @@
       <c r="C25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>32</v>
+      <c r="D25" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="E25" s="16">
         <v>5</v>
@@ -1305,8 +1302,8 @@
       <c r="C26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>104</v>
+      <c r="D26" s="26" t="s">
+        <v>110</v>
       </c>
       <c r="E26" s="16">
         <v>5</v>
@@ -1322,8 +1319,8 @@
       <c r="C27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>33</v>
+      <c r="D27" s="26" t="s">
+        <v>111</v>
       </c>
       <c r="E27" s="16">
         <v>5</v>
@@ -1339,9 +1336,7 @@
       <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="D28" s="26"/>
       <c r="E28" s="16">
         <v>5</v>
       </c>
@@ -1356,9 +1351,7 @@
       <c r="C29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="D29" s="26"/>
       <c r="E29" s="16">
         <v>5</v>
       </c>
@@ -1373,9 +1366,7 @@
       <c r="C30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="D30" s="27"/>
       <c r="E30" s="17">
         <v>6</v>
       </c>
@@ -1390,9 +1381,7 @@
       <c r="C31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>105</v>
-      </c>
+      <c r="D31" s="27"/>
       <c r="E31" s="17">
         <v>6</v>
       </c>
@@ -1407,8 +1396,8 @@
       <c r="C32" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>106</v>
+      <c r="D32" s="27">
+        <v>35</v>
       </c>
       <c r="E32" s="17">
         <v>6</v>
@@ -1424,8 +1413,8 @@
       <c r="C33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>107</v>
+      <c r="D33" s="27">
+        <v>40</v>
       </c>
       <c r="E33" s="17">
         <v>6</v>
@@ -1441,8 +1430,8 @@
       <c r="C34" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>44</v>
+      <c r="D34" s="27">
+        <v>37</v>
       </c>
       <c r="E34" s="17">
         <v>6</v>
@@ -1458,8 +1447,8 @@
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>1</v>
+      <c r="D35" s="28">
+        <v>46</v>
       </c>
       <c r="E35" s="18">
         <v>7</v>
@@ -1475,8 +1464,8 @@
       <c r="C36" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>108</v>
+      <c r="D36" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="E36" s="18">
         <v>7</v>
@@ -1492,8 +1481,8 @@
       <c r="C37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>58</v>
+      <c r="D37" s="28">
+        <v>41</v>
       </c>
       <c r="E37" s="18">
         <v>7</v>
@@ -1509,9 +1498,7 @@
       <c r="C38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>99</v>
-      </c>
+      <c r="D38" s="28"/>
       <c r="E38" s="18">
         <v>7</v>
       </c>
@@ -1526,9 +1513,7 @@
       <c r="C39" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="D39" s="28"/>
       <c r="E39" s="18">
         <v>7</v>
       </c>
@@ -1543,9 +1528,7 @@
       <c r="C40" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="D40" s="29"/>
       <c r="E40" s="19">
         <v>8</v>
       </c>
@@ -1560,9 +1543,7 @@
       <c r="C41" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>66</v>
-      </c>
+      <c r="D41" s="29"/>
       <c r="E41" s="19">
         <v>8</v>
       </c>
@@ -1577,9 +1558,7 @@
       <c r="C42" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="D42" s="29"/>
       <c r="E42" s="19">
         <v>8</v>
       </c>
@@ -1594,8 +1573,8 @@
       <c r="C43" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>109</v>
+      <c r="D43" s="29">
+        <v>46</v>
       </c>
       <c r="E43" s="19">
         <v>8</v>
@@ -1611,9 +1590,7 @@
       <c r="C44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>99</v>
-      </c>
+      <c r="D44" s="29"/>
       <c r="E44" s="19">
         <v>8</v>
       </c>
@@ -1628,9 +1605,7 @@
       <c r="C45" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="D45" s="30"/>
       <c r="E45" s="20">
         <v>9</v>
       </c>
@@ -1645,9 +1620,7 @@
       <c r="C46" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="D46" s="30"/>
       <c r="E46" s="20">
         <v>9</v>
       </c>
@@ -1662,9 +1635,7 @@
       <c r="C47" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="D47" s="30"/>
       <c r="E47" s="20">
         <v>9</v>
       </c>
@@ -1679,8 +1650,8 @@
       <c r="C48" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>110</v>
+      <c r="D48" s="30">
+        <v>51</v>
       </c>
       <c r="E48" s="20">
         <v>9</v>
@@ -1696,9 +1667,7 @@
       <c r="C49" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="D49" s="30"/>
       <c r="E49" s="20">
         <v>9</v>
       </c>
@@ -1713,9 +1682,7 @@
       <c r="C50" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="10" t="s">
-        <v>113</v>
-      </c>
+      <c r="D50" s="31"/>
       <c r="E50" s="21">
         <v>10</v>
       </c>
@@ -1730,9 +1697,7 @@
       <c r="C51" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>113</v>
-      </c>
+      <c r="D51" s="31"/>
       <c r="E51" s="21">
         <v>10</v>
       </c>
@@ -1747,9 +1712,7 @@
       <c r="C52" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>113</v>
-      </c>
+      <c r="D52" s="31"/>
       <c r="E52" s="21">
         <v>10</v>
       </c>
@@ -1764,9 +1727,7 @@
       <c r="C53" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="D53" s="31"/>
       <c r="E53" s="21">
         <v>10</v>
       </c>
@@ -1781,9 +1742,7 @@
       <c r="C54" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>113</v>
-      </c>
+      <c r="D54" s="31"/>
       <c r="E54" s="21">
         <v>10</v>
       </c>
@@ -1791,5 +1750,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D4" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creacion del grafo con los vertices, y comienzo de implementación de las 4 condiciones
</commit_message>
<xml_diff>
--- a/generador ruta critica/MallaCurricular.xlsx
+++ b/generador ruta critica/MallaCurricular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador ruta critica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E32148-5239-4318-9842-32E44E7E1F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8ADAB3-3BEA-4D77-865B-7498CFF56442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -520,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -533,16 +533,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -552,7 +542,27 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -882,7 +892,7 @@
   <dimension ref="A2:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,6 +902,7 @@
     <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,10 +932,10 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="12">
         <v>6</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="21">
         <v>1</v>
       </c>
     </row>
@@ -938,10 +949,10 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="21">
         <v>1</v>
       </c>
     </row>
@@ -955,8 +966,10 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="12">
+      <c r="D5" s="41">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21">
         <v>1</v>
       </c>
     </row>
@@ -970,10 +983,10 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="12">
         <v>9</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="21">
         <v>1</v>
       </c>
     </row>
@@ -987,10 +1000,10 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="12">
         <v>38</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1004,10 +1017,10 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1021,10 +1034,10 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1038,10 +1051,10 @@
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="13">
         <v>13</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1055,10 +1068,10 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1072,8 +1085,10 @@
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="13">
+      <c r="D12" s="32">
+        <v>0</v>
+      </c>
+      <c r="E12" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1087,10 +1102,10 @@
       <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="14">
         <v>18</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1104,10 +1119,10 @@
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1121,8 +1136,10 @@
       <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="14">
+      <c r="D15" s="40">
+        <v>0</v>
+      </c>
+      <c r="E15" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1136,10 +1153,10 @@
       <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="14">
         <v>19</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1153,10 +1170,10 @@
       <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1170,10 +1187,10 @@
       <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1187,8 +1204,10 @@
       <c r="C19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="15">
+      <c r="D19" s="39">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1202,10 +1221,10 @@
       <c r="C20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="15">
         <v>23</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1219,10 +1238,10 @@
       <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1236,8 +1255,10 @@
       <c r="C22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="15">
+      <c r="D22" s="39">
+        <v>0</v>
+      </c>
+      <c r="E22" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1251,10 +1272,10 @@
       <c r="C23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="15">
         <v>27</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1268,10 +1289,10 @@
       <c r="C24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="16">
         <v>29</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1285,10 +1306,10 @@
       <c r="C25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1302,10 +1323,10 @@
       <c r="C26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1319,10 +1340,10 @@
       <c r="C27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1336,8 +1357,10 @@
       <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="16">
+      <c r="D28" s="37">
+        <v>0</v>
+      </c>
+      <c r="E28" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1351,8 +1374,10 @@
       <c r="C29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="16">
+      <c r="D29" s="37">
+        <v>0</v>
+      </c>
+      <c r="E29" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1366,8 +1391,10 @@
       <c r="C30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="17">
+      <c r="D30" s="38">
+        <v>0</v>
+      </c>
+      <c r="E30" s="26">
         <v>6</v>
       </c>
     </row>
@@ -1381,8 +1408,10 @@
       <c r="C31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="17">
+      <c r="D31" s="38">
+        <v>0</v>
+      </c>
+      <c r="E31" s="26">
         <v>6</v>
       </c>
     </row>
@@ -1396,10 +1425,10 @@
       <c r="C32" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="17">
         <v>35</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="26">
         <v>6</v>
       </c>
     </row>
@@ -1413,10 +1442,10 @@
       <c r="C33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="17">
         <v>40</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="26">
         <v>6</v>
       </c>
     </row>
@@ -1430,10 +1459,10 @@
       <c r="C34" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="17">
         <v>37</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="26">
         <v>6</v>
       </c>
     </row>
@@ -1447,10 +1476,10 @@
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="18">
         <v>46</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="27">
         <v>7</v>
       </c>
     </row>
@@ -1464,10 +1493,10 @@
       <c r="C36" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="27">
         <v>7</v>
       </c>
     </row>
@@ -1481,10 +1510,10 @@
       <c r="C37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="18">
         <v>41</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="27">
         <v>7</v>
       </c>
     </row>
@@ -1498,8 +1527,10 @@
       <c r="C38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="18">
+      <c r="D38" s="36">
+        <v>0</v>
+      </c>
+      <c r="E38" s="27">
         <v>7</v>
       </c>
     </row>
@@ -1513,8 +1544,10 @@
       <c r="C39" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="18">
+      <c r="D39" s="36">
+        <v>0</v>
+      </c>
+      <c r="E39" s="27">
         <v>7</v>
       </c>
     </row>
@@ -1528,8 +1561,10 @@
       <c r="C40" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="19">
+      <c r="D40" s="31">
+        <v>0</v>
+      </c>
+      <c r="E40" s="28">
         <v>8</v>
       </c>
     </row>
@@ -1543,8 +1578,10 @@
       <c r="C41" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="19">
+      <c r="D41" s="31">
+        <v>0</v>
+      </c>
+      <c r="E41" s="28">
         <v>8</v>
       </c>
     </row>
@@ -1558,8 +1595,10 @@
       <c r="C42" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="29"/>
-      <c r="E42" s="19">
+      <c r="D42" s="31">
+        <v>0</v>
+      </c>
+      <c r="E42" s="28">
         <v>8</v>
       </c>
     </row>
@@ -1573,10 +1612,10 @@
       <c r="C43" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="19">
         <v>46</v>
       </c>
-      <c r="E43" s="19">
+      <c r="E43" s="28">
         <v>8</v>
       </c>
     </row>
@@ -1590,8 +1629,10 @@
       <c r="C44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="19">
+      <c r="D44" s="31">
+        <v>0</v>
+      </c>
+      <c r="E44" s="28">
         <v>8</v>
       </c>
     </row>
@@ -1605,8 +1646,10 @@
       <c r="C45" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="20">
+      <c r="D45" s="35">
+        <v>0</v>
+      </c>
+      <c r="E45" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1620,8 +1663,10 @@
       <c r="C46" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="20">
+      <c r="D46" s="35">
+        <v>0</v>
+      </c>
+      <c r="E46" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1635,8 +1680,10 @@
       <c r="C47" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="20">
+      <c r="D47" s="35">
+        <v>0</v>
+      </c>
+      <c r="E47" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1650,10 +1697,10 @@
       <c r="C48" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D48" s="30">
+      <c r="D48" s="20">
         <v>51</v>
       </c>
-      <c r="E48" s="20">
+      <c r="E48" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1667,8 +1714,10 @@
       <c r="C49" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="30"/>
-      <c r="E49" s="20">
+      <c r="D49" s="35">
+        <v>0</v>
+      </c>
+      <c r="E49" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1682,8 +1731,10 @@
       <c r="C50" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="21">
+      <c r="D50" s="34">
+        <v>0</v>
+      </c>
+      <c r="E50" s="30">
         <v>10</v>
       </c>
     </row>
@@ -1697,8 +1748,10 @@
       <c r="C51" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="21">
+      <c r="D51" s="34">
+        <v>0</v>
+      </c>
+      <c r="E51" s="30">
         <v>10</v>
       </c>
     </row>
@@ -1712,8 +1765,10 @@
       <c r="C52" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="21">
+      <c r="D52" s="34">
+        <v>0</v>
+      </c>
+      <c r="E52" s="30">
         <v>10</v>
       </c>
     </row>
@@ -1727,8 +1782,10 @@
       <c r="C53" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="31"/>
-      <c r="E53" s="21">
+      <c r="D53" s="34">
+        <v>0</v>
+      </c>
+      <c r="E53" s="30">
         <v>10</v>
       </c>
     </row>
@@ -1742,8 +1799,10 @@
       <c r="C54" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="31"/>
-      <c r="E54" s="21">
+      <c r="D54" s="34">
+        <v>0</v>
+      </c>
+      <c r="E54" s="30">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se terminan las condiciones. Falta refinar detalles
</commit_message>
<xml_diff>
--- a/generador ruta critica/MallaCurricular.xlsx
+++ b/generador ruta critica/MallaCurricular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador ruta critica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8ADAB3-3BEA-4D77-865B-7498CFF56442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7D502-72AD-4BA7-8297-DC8299E07CE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -542,16 +542,6 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -563,6 +553,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -892,7 +892,7 @@
   <dimension ref="A2:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
       <c r="D3" s="12">
         <v>6</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="32">
         <v>1</v>
       </c>
     </row>
@@ -952,7 +952,7 @@
       <c r="D4" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="32">
         <v>1</v>
       </c>
     </row>
@@ -966,10 +966,10 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="41">
-        <v>0</v>
-      </c>
-      <c r="E5" s="21">
+      <c r="D5" s="31">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
         <v>1</v>
       </c>
     </row>
@@ -986,7 +986,7 @@
       <c r="D6" s="12">
         <v>9</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       <c r="D7" s="12">
         <v>38</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       <c r="D8" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       <c r="D9" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       <c r="D10" s="13">
         <v>13</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       <c r="D11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1085,10 +1085,10 @@
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="32">
-        <v>0</v>
-      </c>
-      <c r="E12" s="22">
+      <c r="D12" s="22">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1105,7 +1105,7 @@
       <c r="D13" s="14">
         <v>18</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       <c r="D14" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1136,10 +1136,10 @@
       <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="40">
-        <v>0</v>
-      </c>
-      <c r="E15" s="23">
+      <c r="D15" s="30">
+        <v>0</v>
+      </c>
+      <c r="E15" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       <c r="D16" s="14">
         <v>19</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       <c r="D17" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1190,7 +1190,7 @@
       <c r="D18" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1204,10 +1204,10 @@
       <c r="C19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="39">
-        <v>0</v>
-      </c>
-      <c r="E19" s="24">
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       <c r="D20" s="15">
         <v>23</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       <c r="D21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1255,10 +1255,10 @@
       <c r="C22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="39">
-        <v>0</v>
-      </c>
-      <c r="E22" s="24">
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1275,7 +1275,7 @@
       <c r="D23" s="15">
         <v>27</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1292,7 +1292,7 @@
       <c r="D24" s="16">
         <v>29</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1306,10 +1306,10 @@
       <c r="C25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       <c r="D26" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       <c r="D27" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1357,10 +1357,10 @@
       <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="37">
-        <v>0</v>
-      </c>
-      <c r="E28" s="25">
+      <c r="D28" s="27">
+        <v>0</v>
+      </c>
+      <c r="E28" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1374,10 +1374,10 @@
       <c r="C29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="37">
-        <v>0</v>
-      </c>
-      <c r="E29" s="25">
+      <c r="D29" s="27">
+        <v>0</v>
+      </c>
+      <c r="E29" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1391,10 +1391,10 @@
       <c r="C30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="38">
-        <v>0</v>
-      </c>
-      <c r="E30" s="26">
+      <c r="D30" s="28">
+        <v>0</v>
+      </c>
+      <c r="E30" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1408,10 +1408,10 @@
       <c r="C31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="38">
-        <v>0</v>
-      </c>
-      <c r="E31" s="26">
+      <c r="D31" s="28">
+        <v>0</v>
+      </c>
+      <c r="E31" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1428,7 +1428,7 @@
       <c r="D32" s="17">
         <v>35</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
       <c r="D33" s="17">
         <v>40</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
       <c r="D34" s="17">
         <v>37</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       <c r="D35" s="18">
         <v>46</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
       <c r="D36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="27">
+      <c r="E36" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       <c r="D37" s="18">
         <v>41</v>
       </c>
-      <c r="E37" s="27">
+      <c r="E37" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1527,10 +1527,10 @@
       <c r="C38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="36">
-        <v>0</v>
-      </c>
-      <c r="E38" s="27">
+      <c r="D38" s="26">
+        <v>0</v>
+      </c>
+      <c r="E38" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1544,10 +1544,10 @@
       <c r="C39" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="36">
-        <v>0</v>
-      </c>
-      <c r="E39" s="27">
+      <c r="D39" s="26">
+        <v>0</v>
+      </c>
+      <c r="E39" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1561,10 +1561,10 @@
       <c r="C40" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="31">
-        <v>0</v>
-      </c>
-      <c r="E40" s="28">
+      <c r="D40" s="21">
+        <v>0</v>
+      </c>
+      <c r="E40" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1578,10 +1578,10 @@
       <c r="C41" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="31">
-        <v>0</v>
-      </c>
-      <c r="E41" s="28">
+      <c r="D41" s="21">
+        <v>0</v>
+      </c>
+      <c r="E41" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1595,10 +1595,10 @@
       <c r="C42" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="31">
-        <v>0</v>
-      </c>
-      <c r="E42" s="28">
+      <c r="D42" s="21">
+        <v>0</v>
+      </c>
+      <c r="E42" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       <c r="D43" s="19">
         <v>46</v>
       </c>
-      <c r="E43" s="28">
+      <c r="E43" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1629,10 +1629,10 @@
       <c r="C44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="31">
-        <v>0</v>
-      </c>
-      <c r="E44" s="28">
+      <c r="D44" s="21">
+        <v>0</v>
+      </c>
+      <c r="E44" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1646,10 +1646,10 @@
       <c r="C45" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="35">
-        <v>0</v>
-      </c>
-      <c r="E45" s="29">
+      <c r="D45" s="25">
+        <v>0</v>
+      </c>
+      <c r="E45" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1663,10 +1663,10 @@
       <c r="C46" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="35">
-        <v>0</v>
-      </c>
-      <c r="E46" s="29">
+      <c r="D46" s="25">
+        <v>0</v>
+      </c>
+      <c r="E46" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1680,10 +1680,10 @@
       <c r="C47" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="35">
-        <v>0</v>
-      </c>
-      <c r="E47" s="29">
+      <c r="D47" s="25">
+        <v>0</v>
+      </c>
+      <c r="E47" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1700,7 +1700,7 @@
       <c r="D48" s="20">
         <v>51</v>
       </c>
-      <c r="E48" s="29">
+      <c r="E48" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1714,10 +1714,10 @@
       <c r="C49" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="35">
-        <v>0</v>
-      </c>
-      <c r="E49" s="29">
+      <c r="D49" s="25">
+        <v>0</v>
+      </c>
+      <c r="E49" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1731,10 +1731,10 @@
       <c r="C50" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="34">
-        <v>0</v>
-      </c>
-      <c r="E50" s="30">
+      <c r="D50" s="24">
+        <v>0</v>
+      </c>
+      <c r="E50" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1748,10 +1748,10 @@
       <c r="C51" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="34">
-        <v>0</v>
-      </c>
-      <c r="E51" s="30">
+      <c r="D51" s="24">
+        <v>0</v>
+      </c>
+      <c r="E51" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1765,10 +1765,10 @@
       <c r="C52" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="34">
-        <v>0</v>
-      </c>
-      <c r="E52" s="30">
+      <c r="D52" s="24">
+        <v>0</v>
+      </c>
+      <c r="E52" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1782,10 +1782,10 @@
       <c r="C53" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="34">
-        <v>0</v>
-      </c>
-      <c r="E53" s="30">
+      <c r="D53" s="24">
+        <v>0</v>
+      </c>
+      <c r="E53" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1799,10 +1799,10 @@
       <c r="C54" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="34">
-        <v>0</v>
-      </c>
-      <c r="E54" s="30">
+      <c r="D54" s="24">
+        <v>0</v>
+      </c>
+      <c r="E54" s="41">
         <v>10</v>
       </c>
     </row>

</xml_diff>